<commit_message>
Added end to end and SAP scripts.
</commit_message>
<xml_diff>
--- a/AutomationFramework/Resources/EOBF Global/TestData/Driver.xlsx
+++ b/AutomationFramework/Resources/EOBF Global/TestData/Driver.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ABMMD9A\git\TestAutomationFramework\AutomationFramework\Resources\EOBF Global\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="1" windowHeight="5650" windowWidth="15200" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15200" windowHeight="5650" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Credentials" r:id="rId1" sheetId="1"/>
-    <sheet name="TestData" r:id="rId2" sheetId="2"/>
-    <sheet name="Test" r:id="rId3" sheetId="3"/>
+    <sheet name="Credentials" sheetId="1" r:id="rId1"/>
+    <sheet name="TestData" sheetId="2" r:id="rId2"/>
+    <sheet name="Test" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="168">
   <si>
     <t>Username</t>
   </si>
@@ -530,16 +530,12 @@
   </si>
   <si>
     <t>Thumbela@8</t>
-  </si>
-  <si>
-    <t>Pass</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -666,26 +662,26 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="1" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="3" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -702,10 +698,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -740,7 +736,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -775,7 +771,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -869,21 +865,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -900,7 +896,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -952,15 +948,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
@@ -968,15 +964,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="7.7265625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="21.1796875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="15.26953125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.36328125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="40.1796875" collapsed="true"/>
+    <col min="1" max="1" width="7.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.26953125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="40.1796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="15" r="1" spans="1:6" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -1018,132 +1014,132 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="A2" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2">
       <formula1>"Chrome,IE,Edge,FireFox"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B2" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
       <formula1>"UAT,QA,SIT"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="E2"/>
-    <hyperlink r:id="rId2" ref="F2"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="F2" r:id="rId2"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DC3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:DB3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="CQ1" workbookViewId="0">
+      <selection activeCell="DB9" sqref="DB9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.1796875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.1796875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="40.1796875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.6328125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="17.6328125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="17.36328125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="18.26953125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="10.54296875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="18.54296875" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="16.7265625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="19.1796875" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="16.81640625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="17.453125" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="13.36328125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="15.6328125" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="9.26953125" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="6.7265625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="8.81640625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="14.453125" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="14.6328125" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="12.1796875" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="8.6328125" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="20.81640625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="11.453125" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="9.1796875" collapsed="true"/>
-    <col min="30" max="31" bestFit="true" customWidth="true" width="10.1796875" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="9.54296875" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="10.1796875" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="10.54296875" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" width="12.54296875" collapsed="true"/>
-    <col min="37" max="38" bestFit="true" customWidth="true" width="10.36328125" collapsed="true"/>
-    <col min="39" max="40" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" width="10.1796875" collapsed="true"/>
-    <col min="42" max="42" bestFit="true" customWidth="true" width="14.08984375" collapsed="true"/>
-    <col min="43" max="43" bestFit="true" customWidth="true" width="15.1796875" collapsed="true"/>
-    <col min="44" max="44" bestFit="true" customWidth="true" width="14.08984375" collapsed="true"/>
-    <col min="45" max="45" bestFit="true" customWidth="true" width="15.1796875" collapsed="true"/>
-    <col min="46" max="46" bestFit="true" customWidth="true" width="10.81640625" collapsed="true"/>
-    <col min="47" max="47" bestFit="true" customWidth="true" width="30.0" collapsed="true"/>
-    <col min="48" max="48" bestFit="true" customWidth="true" width="23.36328125" collapsed="true"/>
-    <col min="49" max="49" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="50" max="50" bestFit="true" customWidth="true" width="17.54296875" collapsed="true"/>
-    <col min="51" max="51" bestFit="true" customWidth="true" width="17.81640625" collapsed="true"/>
-    <col min="52" max="52" bestFit="true" customWidth="true" width="17.08984375" collapsed="true"/>
-    <col min="53" max="53" bestFit="true" customWidth="true" width="17.1796875" collapsed="true"/>
-    <col min="54" max="54" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="55" max="55" bestFit="true" customWidth="true" width="17.54296875" collapsed="true"/>
-    <col min="56" max="56" bestFit="true" customWidth="true" width="17.81640625" collapsed="true"/>
-    <col min="57" max="57" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="58" max="58" bestFit="true" customWidth="true" width="15.26953125" collapsed="true"/>
-    <col min="59" max="60" bestFit="true" customWidth="true" width="13.08984375" collapsed="true"/>
-    <col min="61" max="61" bestFit="true" customWidth="true" width="10.54296875" collapsed="true"/>
-    <col min="62" max="62" bestFit="true" customWidth="true" width="13.453125" collapsed="true"/>
-    <col min="63" max="63" bestFit="true" customWidth="true" width="7.7265625" collapsed="true"/>
-    <col min="64" max="64" bestFit="true" customWidth="true" width="10.54296875" collapsed="true"/>
-    <col min="65" max="65" bestFit="true" customWidth="true" width="16.6328125" collapsed="true"/>
-    <col min="66" max="66" bestFit="true" customWidth="true" width="18.1796875" collapsed="true"/>
-    <col min="67" max="67" bestFit="true" customWidth="true" width="14.7265625" collapsed="true"/>
-    <col min="68" max="68" bestFit="true" customWidth="true" width="13.90625" collapsed="true"/>
-    <col min="69" max="69" bestFit="true" customWidth="true" width="11.26953125" collapsed="true"/>
-    <col min="70" max="70" bestFit="true" customWidth="true" width="11.54296875" collapsed="true"/>
-    <col min="71" max="71" bestFit="true" customWidth="true" width="10.81640625" collapsed="true"/>
-    <col min="72" max="72" bestFit="true" customWidth="true" width="14.81640625" collapsed="true"/>
-    <col min="73" max="73" bestFit="true" customWidth="true" width="4.81640625" collapsed="true"/>
-    <col min="74" max="74" bestFit="true" customWidth="true" width="12.1796875" collapsed="true"/>
-    <col min="75" max="75" bestFit="true" customWidth="true" width="6.1796875" collapsed="true"/>
-    <col min="76" max="76" bestFit="true" customWidth="true" width="9.54296875" collapsed="true"/>
-    <col min="77" max="77" bestFit="true" customWidth="true" width="6.7265625" collapsed="true"/>
-    <col min="78" max="78" bestFit="true" customWidth="true" width="7.7265625" collapsed="true"/>
-    <col min="79" max="79" bestFit="true" customWidth="true" width="9.453125" collapsed="true"/>
-    <col min="80" max="80" bestFit="true" customWidth="true" width="4.36328125" collapsed="true"/>
-    <col min="81" max="81" bestFit="true" customWidth="true" width="6.1796875" collapsed="true"/>
-    <col min="82" max="82" bestFit="true" customWidth="true" width="9.6328125" collapsed="true"/>
-    <col min="83" max="83" bestFit="true" customWidth="true" width="4.54296875" collapsed="true"/>
-    <col min="84" max="84" bestFit="true" customWidth="true" width="4.6328125" collapsed="true"/>
-    <col min="85" max="85" bestFit="true" customWidth="true" width="9.81640625" collapsed="true"/>
-    <col min="86" max="86" bestFit="true" customWidth="true" width="19.54296875" collapsed="true"/>
-    <col min="87" max="87" bestFit="true" customWidth="true" width="14.08984375" collapsed="true"/>
-    <col min="88" max="88" bestFit="true" customWidth="true" width="19.08984375" collapsed="true"/>
-    <col min="89" max="89" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="90" max="90" bestFit="true" customWidth="true" width="9.81640625" collapsed="true"/>
-    <col min="91" max="91" bestFit="true" customWidth="true" width="15.26953125" collapsed="true"/>
-    <col min="92" max="92" bestFit="true" customWidth="true" width="45.36328125" collapsed="true"/>
-    <col min="93" max="93" bestFit="true" customWidth="true" width="9.54296875" collapsed="true"/>
-    <col min="94" max="94" bestFit="true" customWidth="true" width="8.6328125" collapsed="true"/>
-    <col min="95" max="95" bestFit="true" customWidth="true" width="9.453125" collapsed="true"/>
-    <col min="96" max="96" bestFit="true" customWidth="true" width="18.08984375" collapsed="true"/>
-    <col min="97" max="97" bestFit="true" customWidth="true" width="18.54296875" collapsed="true"/>
-    <col min="98" max="98" bestFit="true" customWidth="true" width="10.26953125" collapsed="true"/>
-    <col min="99" max="99" bestFit="true" customWidth="true" width="14.54296875" collapsed="true"/>
-    <col min="100" max="100" bestFit="true" customWidth="true" width="14.1796875" collapsed="true"/>
-    <col min="101" max="101" bestFit="true" customWidth="true" width="11.81640625" collapsed="true"/>
-    <col min="102" max="102" bestFit="true" customWidth="true" width="10.1796875" collapsed="true"/>
-    <col min="103" max="103" bestFit="true" customWidth="true" width="16.453125" collapsed="true"/>
-    <col min="105" max="105" bestFit="true" customWidth="true" width="17.26953125" collapsed="true"/>
-    <col min="106" max="106" bestFit="true" customWidth="true" width="14.36328125" collapsed="true"/>
+    <col min="1" max="1" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="40.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="18.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="10.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="18.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="16.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="19.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="16.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="17.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="13.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="15.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="9.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="6.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="8.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="14.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="14.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="12.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="8.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="20.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="9.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="31" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="9.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="10.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="38" width="10.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="40" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="14.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="15.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="14.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="15.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="10.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="23.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="17.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="17.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="17.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="17.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="17.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="15.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="60" width="13.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="61" max="61" width="10.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="62" max="62" width="13.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="63" max="63" width="7.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="64" max="64" width="10.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="65" max="65" width="16.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="66" max="66" width="18.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="67" max="67" width="14.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="68" max="68" width="13.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="69" max="69" width="11.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="70" max="70" width="11.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="71" max="71" width="10.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="72" max="72" width="14.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="73" max="73" width="4.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="74" max="74" width="12.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="75" max="75" width="6.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="76" max="76" width="9.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="77" max="77" width="6.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="78" max="78" width="7.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="79" max="79" width="9.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="80" max="80" width="4.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="81" max="81" width="6.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="82" max="82" width="9.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="83" max="83" width="4.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="84" max="84" width="4.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="85" max="85" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="86" max="86" width="19.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="87" max="87" width="14.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="88" max="88" width="19.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="89" max="89" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="90" max="90" width="9.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="91" max="91" width="15.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="92" max="92" width="45.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="93" max="93" width="9.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="94" max="94" width="8.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="95" max="95" width="9.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="96" max="96" width="18.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="97" max="97" width="18.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="98" max="98" width="10.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="99" max="99" width="14.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="100" max="100" width="14.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="101" max="101" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="102" max="102" width="10.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="103" max="103" width="16.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="105" max="105" width="17.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="106" max="106" width="14.36328125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:106" x14ac:dyDescent="0.35">
@@ -1771,11 +1767,9 @@
         <v>#REF!</v>
       </c>
       <c r="DA2" s="5">
-        <v>180162183724433</v>
-      </c>
-      <c r="DB2" s="7" t="s">
-        <v>168</v>
-      </c>
+        <v>180015100438342</v>
+      </c>
+      <c r="DB2" s="7"/>
     </row>
     <row r="3" spans="1:106" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -2084,100 +2078,100 @@
     </row>
   </sheetData>
   <dataValidations count="28">
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B2:B3 AJ2:AJ3 P2:P3 K2:K3 G2:G3 E2:E3 Z2:Z3 BV2:BV3 BW2:CE2 BZ3:CE3 CF2:CG3 CR2:CT3" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B3 AJ2:AJ3 P2:P3 K2:K3 G2:G3 E2:E3 Z2:Z3 BV2:BV3 BW2:CE2 BZ3:CE3 CF2:CG3 CR2:CT3">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="D2:D3" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3">
       <formula1>"Individual,Sole Trader(sole proprieter),Sole Trader(farmer)"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="H2:H3" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H3">
       <formula1>"Mr,Mrs,Miss,Professor,Doctor,Ms,Lord,Advocate"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="L2:L3" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L3">
       <formula1>"Valid Id,Passport"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="S2:S3" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2:S3">
       <formula1>"Male,Female"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="T2:T3" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2:T3">
       <formula1>"African,Indian,Coloured,Indian,White,Asian"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="V2:V3" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2:V3">
       <formula1>"SOUTH AFRICAN,ANGOLAN,FRENCH,SPANISH,DUTCH"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="Y2:Y3" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y2:Y3">
       <formula1>"Afrikaans,English"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="X2:X3" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X2:X3">
       <formula1>"Married,Single,Divoced,Widow/er,Antenuptual Contract,Community of Property"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="AA2:AA3" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA2:AA3">
       <formula1>"Honours,Masters,Doctorate,Degree 3 and 3+ years"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="W2:W3" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W2:W3">
       <formula1>"SOUTH AFRICA,ANGOLA,FRANCE,SPAIN"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="AB2:AB3" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB2:AB3">
       <formula1>"Owner,Tenant,Boarder,Living With Parents"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="AV2:AV3" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AV2:AV3">
       <formula1>"Mail,E-mail,Telephone,SMS"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="AY2:AY3" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AY2:AY3">
       <formula1>"Aunt,Brother,Cousin,Father,Friend,Mother,Husband,Wife,Sister,Life Partner"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="BA2:BA3" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BA2:BA3">
       <formula1>"Full Time Employed,Self Employed Professional,Self Employed Non-Professional,Student,Unemployed,Pensioner,Part Time/Contract Worker,Temporary Employed"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="BB2:BB3" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BB2:BB3">
       <formula1>"Agriculture,Catering and Entertainment,Finance,Health,Science/Computing,Security,Transportation,Other"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="BD2:BD3" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BD2:BD3">
       <formula1>"Senior Management,Management,Supervisor,Skilled Worker,Semi-Skilled Worker,Unskilled Worker,Junior Position"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="BE2:BE3" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BE2:BE3">
       <formula1>"Administration,Architect,Biokenetocist,Chatered Accountant,Dentist,Engineer,Lawyer,Optometrist,Other,Technician,Professional"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="BQ2" type="whole">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BQ2">
       <formula1>1</formula1>
       <formula2>30</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="BO2:BP3" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BO2:BP3">
       <formula1>"Salary/Wages,Commission,Bonus,Maintenance/Alimony,Pension,Investments,Retirement Annuity,Inheritance,Social Grant,Sale of Property,Sale of Vehicle"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="CH2:CH3" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CH2:CH3">
       <formula1>"Instalment Agreement,Lease Agreement,Rental Agreement,Islamic Lease Agreement"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="CI2:CI3" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CI2:CI3">
       <formula1>"Light Duty Vehicle,Motor Vehicle,Motorbikes,Other"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="CJ2:CJ3" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CJ2:CJ3">
       <formula1>"Livestock,Bicycles,Boats,Caravans And Camping Equipment,Trailers,Tractors"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="CL2:CL3" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CL2:CL3">
       <formula1>"2018,2017,2016,2015,2014,2013,2012,2011,2010,2000,1999,1991"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="CO2:CO3" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CO2:CO3">
       <formula1>"50cc &gt;&lt; 251cc,250cc &gt;&lt; 651cc,&gt; 650cc"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="CU2:CU3" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CU2:CU3">
       <formula1>"Absa,Bank of Athens,Bidvest Bank,Capitec Bank,FNB,Private Bank,Nedbank,SA Post Bank,Standard Bank,Other,Investec Private Bank"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="CW2:CW3" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CW2:CW3">
       <formula1>"Cheque,Savings,Transmission"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="CY2:CY3" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CY2:CY3">
       <formula1>"Email,Post"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
@@ -2203,10 +2197,10 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="A2" type="list">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>